<commit_message>
Changed 2-pin terminal block and 7-Segment display suppliers on the BOM. This shaved 30% off the original per-board price.
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -73,13 +73,13 @@
     <t xml:space="preserve">https://www.digikey.com/products/en?keywords=JK0654219NL</t>
   </si>
   <si>
-    <t xml:space="preserve">TE   282837-2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TE Connectivity   2P Terminal Block</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.com/product-detail/en/te-connectivity-amp-connectors/282837-2/A113320-ND/2187973</t>
+    <t xml:space="preserve">DBParts 20 pc 2-pin 0.1” pitch Terminal Blocks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amazon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.amazon.com/DBParts-20pcs-Terminal-Connector-2-54mm/dp/B07NSJV6NW/ref=sxbs_sxwds-stvp?cv_ct_cx=terminal+block+assortment&amp;keywords=terminal+block+assortment&amp;pd_rd_i=B07NSJV6NW&amp;pd_rd_r=f9187fb7-4ab9-45b4-a445-3bf2b68a1d13&amp;pd_rd_w=WAjjn&amp;pd_rd_wg=olYB9&amp;pf_rd_p=a6d018ad-f20b-46c9-8920-433972c7d9b7&amp;pf_rd_r=PMA44C3EHR468DBRJFP7&amp;psc=1&amp;qid=1581446551&amp;sr=1-3-dd5817a1-1ba7-46c2-8996-f96e7b0f409c</t>
   </si>
   <si>
     <t xml:space="preserve">Adafruit 2772</t>
@@ -127,13 +127,13 @@
     <t xml:space="preserve">https://www.digikey.com/product-detail/en/nichicon/UVK2GR47MED1TD/493-12648-3-ND/4328849</t>
   </si>
   <si>
-    <t xml:space="preserve">Lite-On LTS-6760P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Red 7-Segment 10-DIN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.com/product-detail/en/lite-on-inc/LTS-6760P/160-2014-5-ND/3199482</t>
+    <t xml:space="preserve">Uxcell 10 pc 7-Segment 10DIN LED Display</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7-Segment 10-DIN 10 pc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.amazon.com/a13071500ux0900-Cathode-Segment-Display-Digital/dp/B00EZBGUMC/ref=sr_1_fkmr0_1?keywords=7-Segment+10+DIN+LED&amp;qid=1581447942&amp;sr=8-1-fkmr0</t>
   </si>
   <si>
     <t xml:space="preserve">*Discount prices are available for the</t>
@@ -281,13 +281,13 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C14:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.32"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.72"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
@@ -393,22 +393,23 @@
         <v>17</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>1.04</v>
+        <v>6.99</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>1</v>
+        <f aca="false">1/20</f>
+        <v>0.05</v>
       </c>
       <c r="E5" s="2" t="n">
         <f aca="false">C5*D5</f>
-        <v>1.04</v>
+        <v>0.3495</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>19</v>
       </c>
     </row>
@@ -540,17 +541,18 @@
         <v>36</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>1.75</v>
+        <v>5.99</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>9</v>
+        <f aca="false">9/10</f>
+        <v>0.9</v>
       </c>
       <c r="E11" s="2" t="n">
         <f aca="false">C11*D11</f>
-        <v>15.75</v>
+        <v>5.391</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>37</v>
@@ -569,7 +571,7 @@
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E14" s="2" t="n">
         <f aca="false">E2+E3+E4+E5+E6+E7+E8+E9+E10+E11</f>
-        <v>48.46</v>
+        <v>37.4105</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Changed resistor footprints, changed resistor supplier. Still need to route wires.
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -91,22 +91,22 @@
     <t xml:space="preserve">https://www.digikey.com/product-detail/en/adafruit-industries-llc/2772/1528-1531-ND/5775537</t>
   </si>
   <si>
-    <t xml:space="preserve">Vishay Dale CRCW2010100RFKEFHP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Solderable size 2010 100 ohm SMD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.com/product-detail/en/vishay-dale/CRCW2010100RFKEFHP/541-100PCT-ND/2222676</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vishay Dale CRCW201010R0FKEF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Solderable size 2010 10 ohm SMD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.com/product-detail/en/vishay-dale/CRCW201010R0FKEF/541-10.0ACCT-ND/1179050</t>
+    <t xml:space="preserve">Stackpole Electronics RSMF2JT330R </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Through Hole 330 ohm 2 watt resistor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/product-detail/en/stackpole-electronics-inc/RSF2JT330R/RSF2JT330RCT-ND/2021796</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stackpole Electronics  CF12JT10R0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Through Hole 10 ohm ½ watt Resistor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/product-detail/en/stackpole-electronics-inc/CF12JT10R0/CF12JT10R0CT-ND/1830446</t>
   </si>
   <si>
     <t xml:space="preserve">WIMA FKP0D001000B00JSSD</t>
@@ -281,7 +281,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C14:C15"/>
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -445,14 +445,14 @@
         <v>24</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>0.58</v>
+        <v>0.29</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>9</v>
       </c>
       <c r="E7" s="2" t="n">
         <f aca="false">C7*D7</f>
-        <v>5.22</v>
+        <v>2.61</v>
       </c>
       <c r="F7" s="0" t="s">
         <v>9</v>
@@ -469,14 +469,14 @@
         <v>27</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>0.29</v>
+        <v>0.1</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>2</v>
       </c>
       <c r="E8" s="2" t="n">
         <f aca="false">C8*D8</f>
-        <v>0.58</v>
+        <v>0.2</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>9</v>
@@ -571,7 +571,7 @@
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E14" s="2" t="n">
         <f aca="false">E2+E3+E4+E5+E6+E7+E8+E9+E10+E11</f>
-        <v>37.4105</v>
+        <v>34.4205</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Major revisions occurred to the Schematic. Sourced 7-Segment display and MosFETs.
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -307,7 +307,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -316,7 +316,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.85"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="19.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.35"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -488,19 +488,19 @@
         <v>0.32</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E6" s="0" t="n">
-        <f aca="false">_xlfn.CEILING.MATH(5*D6)</f>
-        <v>20</v>
+        <f aca="false">8*_xlfn.CEILING.MATH(20/3)+4*5</f>
+        <v>76</v>
       </c>
       <c r="F6" s="2" t="n">
         <f aca="false">C6*D6</f>
-        <v>1.28</v>
+        <v>3.84</v>
       </c>
       <c r="G6" s="2" t="n">
         <f aca="false">C6*E6</f>
-        <v>6.4</v>
+        <v>24.32</v>
       </c>
       <c r="H6" s="0" t="s">
         <v>11</v>
@@ -749,11 +749,11 @@
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F18" s="2" t="n">
         <f aca="false">F2+F3+F4+F5+F6+F7+F8+F9+F10+F11+F12+F13+F14</f>
-        <v>41.2</v>
+        <v>43.76</v>
       </c>
       <c r="G18" s="2" t="n">
         <f aca="false">G2+G3+G4+G5+G6+G7+G8+G9+G10+G11+G12+G13+G14</f>
-        <v>124.76</v>
+        <v>142.68</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Schematic Finished. Need to figure out geometry and route layout.
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="59">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -91,6 +91,24 @@
     <t xml:space="preserve">https://www.digikey.com/product-detail/en/te-connectivity-amp-connectors/640456-2/A1921-ND/109003</t>
   </si>
   <si>
+    <t xml:space="preserve">TE Connectivity 1-640454-7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONN HEADER VERT 17POS 2.54MM </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/product-detail/en/te-connectivity-amp-connectors/1-640454-7/A112540-ND/1152594</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TE Connectivity 1-102241-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CONN HOUSING 17POS 2.54MM </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/product-detail/en/te-connectivity-amp-connectors/1-102241-5/A111776-ND/2286104</t>
+  </si>
+  <si>
     <t xml:space="preserve">On Semiconductor 2N7000</t>
   </si>
   <si>
@@ -107,6 +125,24 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.digikey.com/product-detail/en/kingbright/SC10-21SRWA/754-1700-5-ND/3084550</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TI CD4511BE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7-Segment Display driver, 16-DIP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/product-detail/en/texas-instruments/CD4511BE/296-2072-ND/67341</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TI CD74HC238E </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3x8 Decoder, 16DIP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/product-detail/en/texas-instruments/CD74HC238E/296-25983-5-ND/1506865</t>
   </si>
   <si>
     <t xml:space="preserve">Adafruit 2772</t>
@@ -304,19 +340,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="47.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.85"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="19.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.36"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -477,304 +513,405 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C6" s="2" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(5*D6)</f>
+        <v>10</v>
+      </c>
+      <c r="F6" s="2" t="n">
+        <f aca="false">C6*D6</f>
+        <v>1.98</v>
+      </c>
+      <c r="G6" s="2" t="n">
+        <f aca="false">C6*E6</f>
+        <v>9.9</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>1.59</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(5*D7)</f>
+        <v>10</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <f aca="false">C7*D7</f>
+        <v>3.18</v>
+      </c>
+      <c r="G7" s="2" t="n">
+        <f aca="false">C7*E7</f>
+        <v>15.9</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="2" t="n">
         <v>0.32</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D8" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E8" s="0" t="n">
         <f aca="false">8*_xlfn.CEILING.MATH(20/3)+4*5</f>
         <v>76</v>
       </c>
-      <c r="F6" s="2" t="n">
-        <f aca="false">C6*D6</f>
+      <c r="F8" s="2" t="n">
+        <f aca="false">C8*D8</f>
         <v>3.84</v>
       </c>
-      <c r="G6" s="2" t="n">
-        <f aca="false">C6*E6</f>
-        <v>24.32</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="2" t="n">
-        <v>3.04</v>
-      </c>
-      <c r="D7" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="E7" s="0" t="n">
-        <f aca="false">_xlfn.CEILING.MATH(5*D7)</f>
-        <v>20</v>
-      </c>
-      <c r="F7" s="2" t="n">
-        <f aca="false">C7*D7</f>
-        <v>12.16</v>
-      </c>
-      <c r="G7" s="2" t="n">
-        <f aca="false">C7*E7</f>
-        <v>60.8</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="I7" s="0" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5"/>
-      <c r="C8" s="2"/>
-      <c r="E8" s="0" t="n">
-        <f aca="false">_xlfn.CEILING.MATH(5*D8)</f>
-        <v>0</v>
-      </c>
-      <c r="F8" s="2"/>
       <c r="G8" s="2" t="n">
         <f aca="false">C8*E8</f>
-        <v>0</v>
+        <v>24.32</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5"/>
-      <c r="C9" s="2"/>
+      <c r="A9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>3.04</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="E9" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(5*D9)</f>
-        <v>0</v>
-      </c>
-      <c r="F9" s="2"/>
+        <v>20</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <f aca="false">C9*D9</f>
+        <v>12.16</v>
+      </c>
       <c r="G9" s="2" t="n">
         <f aca="false">C9*E9</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>29</v>
+        <v>60.8</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>19.95</v>
+        <v>0.46</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E10" s="0" t="n">
+        <f aca="false">1</f>
         <v>1</v>
       </c>
       <c r="F10" s="2" t="n">
         <f aca="false">C10*D10</f>
-        <v>19.95</v>
+        <v>0.46</v>
       </c>
       <c r="G10" s="2" t="n">
         <f aca="false">C10*E10</f>
-        <v>19.95</v>
+        <v>0.46</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>32</v>
+        <v>18</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>0.28</v>
+        <v>0.6</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E11" s="0" t="n">
-        <f aca="false">_xlfn.CEILING.MATH(5*D11)</f>
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="F11" s="2" t="n">
         <f aca="false">C11*D11</f>
-        <v>2.24</v>
+        <v>0.6</v>
       </c>
       <c r="G11" s="2" t="n">
         <f aca="false">C11*E11</f>
-        <v>11.2</v>
+        <v>1.8</v>
       </c>
       <c r="H11" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="I11" s="3" t="s">
-        <v>34</v>
+      <c r="I11" s="0" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C12" s="2" t="n">
-        <v>0.1</v>
+        <v>19.95</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E12" s="0" t="n">
-        <f aca="false">_xlfn.CEILING.MATH(5*D12)</f>
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="F12" s="2" t="n">
         <f aca="false">C12*D12</f>
-        <v>0.4</v>
+        <v>19.95</v>
       </c>
       <c r="G12" s="2" t="n">
         <f aca="false">C12*E12</f>
-        <v>2</v>
+        <v>19.95</v>
       </c>
       <c r="H12" s="0" t="s">
         <v>11</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C13" s="2" t="n">
-        <v>0.24</v>
+        <v>0.28</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E13" s="0" t="n">
-        <f aca="false">_xlfn.CEILING.MATH(3*D13)</f>
-        <v>9</v>
+        <f aca="false">_xlfn.CEILING.MATH(5*D13)</f>
+        <v>40</v>
       </c>
       <c r="F13" s="2" t="n">
         <f aca="false">C13*D13</f>
-        <v>0.72</v>
+        <v>2.24</v>
       </c>
       <c r="G13" s="2" t="n">
         <f aca="false">C13*E13</f>
-        <v>2.16</v>
+        <v>11.2</v>
       </c>
       <c r="H13" s="0" t="s">
         <v>11</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C14" s="2" t="n">
-        <v>0.06</v>
+        <v>0.1</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E14" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(5*D14)</f>
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="F14" s="2" t="n">
         <f aca="false">C14*D14</f>
-        <v>0.06</v>
+        <v>0.4</v>
       </c>
       <c r="G14" s="2" t="n">
         <f aca="false">C14*E14</f>
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="H14" s="0" t="s">
         <v>11</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="I15" s="3"/>
+      <c r="A15" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(3*D15)</f>
+        <v>9</v>
+      </c>
+      <c r="F15" s="2" t="n">
+        <f aca="false">C15*D15</f>
+        <v>0.72</v>
+      </c>
+      <c r="G15" s="2" t="n">
+        <f aca="false">C15*E15</f>
+        <v>2.16</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="I16" s="3"/>
+      <c r="A16" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(5*D16)</f>
+        <v>5</v>
+      </c>
+      <c r="F16" s="2" t="n">
+        <f aca="false">C16*D16</f>
+        <v>0.06</v>
+      </c>
+      <c r="G16" s="2" t="n">
+        <f aca="false">C16*E16</f>
+        <v>0.3</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F17" s="6" t="s">
+      <c r="C17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="I17" s="3"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="I18" s="3"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F19" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="G19" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F18" s="2" t="n">
-        <f aca="false">F2+F3+F4+F5+F6+F7+F8+F9+F10+F11+F12+F13+F14</f>
-        <v>43.76</v>
-      </c>
-      <c r="G18" s="2" t="n">
-        <f aca="false">G2+G3+G4+G5+G6+G7+G8+G9+G10+G11+G12+G13+G14</f>
-        <v>142.68</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F19" s="0" t="s">
-        <v>44</v>
-      </c>
-    </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F20" s="0" t="s">
-        <v>45</v>
+      <c r="F20" s="2" t="n">
+        <f aca="false">F2+F3+F4+F5+F6+F7+F8+F9+F10+F11+F12+F13+F14+F15+F16</f>
+        <v>49.98</v>
+      </c>
+      <c r="G20" s="2" t="n">
+        <f aca="false">G2+G3+G4+G5+G6+G7+G8+G9+G10+G11+G12+G13+G14+G15+G16</f>
+        <v>170.74</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F21" s="0" t="s">
-        <v>46</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F22" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F23" s="0" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1" display="https://www.digikey.com/product-detail/en/texas-instruments/SN65HVD72DR/296-39179-1-ND/5143186"/>
-    <hyperlink ref="I10" r:id="rId2" display="https://www.digikey.com/product-detail/en/adafruit-industries-llc/2772/1528-1531-ND/5775537"/>
+    <hyperlink ref="I12" r:id="rId2" display="https://www.digikey.com/product-detail/en/adafruit-industries-llc/2772/1528-1531-ND/5775537"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>